<commit_message>
Fix fund code in config list
</commit_message>
<xml_diff>
--- a/config/科创债名单.xlsx
+++ b/config/科创债名单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\bond-etf-auto\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1C89D2-ED00-42CE-AE03-AEB44A2FE449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB2D790-CB19-4BC4-96C1-F3D1A55D7242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4488" yWindow="-17388" windowWidth="30936" windowHeight="16776" xr2:uid="{FD561B31-178A-40A3-B68B-FAEB2496E593}"/>
   </bookViews>
@@ -87,9 +87,6 @@
     <t>科创债ETF大成</t>
   </si>
   <si>
-    <t>科创债ETF平安</t>
-  </si>
-  <si>
     <t>科创债ETF华安</t>
   </si>
   <si>
@@ -103,13 +100,17 @@
   </si>
   <si>
     <t>科创债ETF南方</t>
+  </si>
+  <si>
+    <t>科创债ETF景顺</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,6 +145,14 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -183,7 +192,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -194,6 +203,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -513,7 +525,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -694,8 +706,8 @@
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>20</v>
+      <c r="A20" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="B20" s="1">
         <v>159400</v>
@@ -704,7 +716,7 @@
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1">
         <v>159115</v>
@@ -713,7 +725,7 @@
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1">
         <v>159116</v>
@@ -722,7 +734,7 @@
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1">
         <v>159200</v>
@@ -731,7 +743,7 @@
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1">
         <v>159600</v>
@@ -740,7 +752,7 @@
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1">
         <v>159700</v>

</xml_diff>